<commit_message>
added archive  noescape scrap
</commit_message>
<xml_diff>
--- a/noescape_scrap_newcommers_data.xlsx
+++ b/noescape_scrap_newcommers_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,16 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>attack_information</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>total_data</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>publish_date</t>
         </is>
       </c>
     </row>
@@ -518,6 +528,16 @@
 </t>
         </is>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>70 GB</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>25 Sep 2023</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -562,6 +582,16 @@
 </t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>80.68 KB</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>25 Sep 2023</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -604,6 +634,16 @@
 Assign a person to the position of negotiator, and tell him to contact us, we will explain everything and help you solve this problem.
 Time is running out.
 </t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>191.62 KB</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>20 Sep 2023</t>
         </is>
       </c>
     </row>
@@ -659,6 +699,16 @@
 </t>
         </is>
       </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1.64 MB</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>17 Sep 2023</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -701,6 +751,16 @@
 Assign a person to the position of negotiator, and tell him to contact us, we will explain everything and help you solve this problem.
 Time is running out.
 </t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>804.51 KB</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>16 Sep 2023</t>
         </is>
       </c>
     </row>
@@ -754,6 +814,16 @@
 </t>
         </is>
       </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>594.16 KB</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>14 Sep 2023</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -802,6 +872,16 @@
 </t>
         </is>
       </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>496.55 KB</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>10 Sep 2023</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -848,6 +928,16 @@
 If you guys don’t contact us before the end of the timer, and don’t start negotiations on the price that we told you and continue to offer pennies, then all the data will be published.
 Time is running out.
 </t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>415.42 KB</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>10 Sep 2023</t>
         </is>
       </c>
     </row>
@@ -902,6 +992,16 @@
 </t>
         </is>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>873.62 KB</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>21 Sep 2023</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -943,6 +1043,16 @@
 Assign a person to the position of negotiator, and tell him to contact us, we will explain everything and help you solve this problem.
 Time is running out.
 </t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>17 GB</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>24 Sep 2023</t>
         </is>
       </c>
     </row>
@@ -990,6 +1100,16 @@
 </t>
         </is>
       </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>25 GB</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>24 Sep 2023</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1032,6 +1152,16 @@
 Assign a person to the position of negotiator, and tell him to contact us, we will explain everything and help you solve this problem.
 Time is running out.
 </t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>20 GB</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>24 Sep 2023</t>
         </is>
       </c>
     </row>
@@ -1083,6 +1213,16 @@
 </t>
         </is>
       </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>218.02 KB</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>20 Sep 2023</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>